<commit_message>
built simple vhdl file for seven segment display
</commit_message>
<xml_diff>
--- a/Design Data.xlsx
+++ b/Design Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clarkson College\EE 365\EE365_secrurity_system_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C60CC7-9F83-49F3-89DA-E1F2182FEA1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9852D232-A784-480E-9D1E-3B4DA1BCFC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3996" yWindow="1248" windowWidth="11064" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
   <si>
     <t>Column 1</t>
   </si>
@@ -97,6 +97,138 @@
   </si>
   <si>
     <t>010000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>IO1</t>
+  </si>
+  <si>
+    <t>IO0</t>
+  </si>
+  <si>
+    <t>IO2</t>
+  </si>
+  <si>
+    <t>IO3</t>
+  </si>
+  <si>
+    <t>IO4</t>
+  </si>
+  <si>
+    <t>IO5</t>
+  </si>
+  <si>
+    <t>IO6</t>
+  </si>
+  <si>
+    <t>IO7</t>
+  </si>
+  <si>
+    <t>IO8</t>
+  </si>
+  <si>
+    <t>IO9</t>
+  </si>
+  <si>
+    <t>IO10</t>
+  </si>
+  <si>
+    <t>IO11</t>
+  </si>
+  <si>
+    <t>IO12</t>
+  </si>
+  <si>
+    <t>IO26</t>
+  </si>
+  <si>
+    <t>IO27</t>
+  </si>
+  <si>
+    <t>IO28</t>
+  </si>
+  <si>
+    <t>Select GND/IO13</t>
+  </si>
+  <si>
+    <t>Select GND/IO29</t>
+  </si>
+  <si>
+    <t>Select GND/IO30</t>
+  </si>
+  <si>
+    <t>Select GND/IO31</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>DIG2</t>
+  </si>
+  <si>
+    <t>DIG3</t>
+  </si>
+  <si>
+    <t>DIG1</t>
+  </si>
+  <si>
+    <t>DIG4</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -426,138 +558,420 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:K6"/>
+  <dimension ref="B2:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="2"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="1">
+        <v>7</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="1">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="1">
+        <v>9</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="1">
+        <v>10</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="1">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="1">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
modified seven segment driver
</commit_message>
<xml_diff>
--- a/Design Data.xlsx
+++ b/Design Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Clarkson College\EE 365\EE365_secrurity_system_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9852D232-A784-480E-9D1E-3B4DA1BCFC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83DAAD2-6AD9-4644-88E3-DF48F6737660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3996" yWindow="1248" windowWidth="11064" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2508" windowWidth="11064" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="83">
   <si>
     <t>Column 1</t>
   </si>
@@ -229,6 +229,51 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>SEG_SEL[0]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[1]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[2]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[3]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[4]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[5]</t>
+  </si>
+  <si>
+    <t>SEG_SEL[6]</t>
+  </si>
+  <si>
+    <t>GND_CTRL_VEC[0]</t>
+  </si>
+  <si>
+    <t>GND_CTRL_VEC[1]</t>
+  </si>
+  <si>
+    <t>GND_CTRL_VEC[2]</t>
+  </si>
+  <si>
+    <t>GND_CTRL_VEC[3]</t>
+  </si>
+  <si>
+    <t>IO29</t>
+  </si>
+  <si>
+    <t>IO30</t>
+  </si>
+  <si>
+    <t>IO31</t>
+  </si>
+  <si>
+    <t>IO32</t>
   </si>
 </sst>
 </file>
@@ -561,14 +606,16 @@
   <dimension ref="B2:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="6" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
@@ -851,8 +898,17 @@
       <c r="D16" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>2</v>
       </c>
@@ -862,8 +918,17 @@
       <c r="D17" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>3</v>
       </c>
@@ -873,8 +938,14 @@
       <c r="D18" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="F18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>4</v>
       </c>
@@ -884,8 +955,17 @@
       <c r="D19" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>5</v>
       </c>
@@ -895,8 +975,17 @@
       <c r="D20" s="1" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>6</v>
       </c>
@@ -906,8 +995,17 @@
       <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>7</v>
       </c>
@@ -917,8 +1015,17 @@
       <c r="D22" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>8</v>
       </c>
@@ -928,8 +1035,17 @@
       <c r="D23" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E23" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>9</v>
       </c>
@@ -939,8 +1055,17 @@
       <c r="D24" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>10</v>
       </c>
@@ -950,8 +1075,17 @@
       <c r="D25" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>11</v>
       </c>
@@ -961,8 +1095,17 @@
       <c r="D26" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>12</v>
       </c>
@@ -971,6 +1114,9 @@
       </c>
       <c r="D27" s="1" t="s">
         <v>64</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>